<commit_message>
feat: add severity field, handleErrorByCode, and enhanced Sentry plugin
- Add severity field (INFO/WARNING/ERROR/CRITICAL) to core schema, parser,
  validator, and all framework bindings (React/Vue/Svelte)
- Add handleErrorByCode with errorMap and fallbackTrackId to all framework
  providers for error code→trackId mapping
- Enhance Sentry plugin with severity-based level mapping, ignoreTypes,
  ignoreTrackIds, sensitiveKeys masking, urlPatterns fingerprinting, and
  enrichContext callback
- Update templates (CSV/XLSX/Airtable/Notion/Google Sheets) with severity
  field and fix Notion schema update for existing databases
- Add field ordering warning for Airtable existing base updates
- Update all documentation (ko/en) and example configs

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/scripts/templates/output/huh-template.xlsx
+++ b/scripts/templates/output/huh-template.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -408,9 +408,10 @@
     <col min="3" max="3" width="28.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -430,12 +431,15 @@
         <v>image</v>
       </c>
       <c r="F1" t="str">
+        <v>severity</v>
+      </c>
+      <c r="G1" t="str">
         <v>actionLabel</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>actionType</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>actionTarget</v>
       </c>
     </row>
@@ -456,12 +460,15 @@
         <v/>
       </c>
       <c r="F2" t="str">
+        <v>WARNING</v>
+      </c>
+      <c r="G2" t="str">
         <v>다시 시도</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" t="str">
         <v>RETRY</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
         <v/>
       </c>
     </row>
@@ -482,12 +489,15 @@
         <v/>
       </c>
       <c r="F3" t="str">
+        <v>ERROR</v>
+      </c>
+      <c r="G3" t="str">
         <v>로그인</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" t="str">
         <v>REDIRECT</v>
       </c>
-      <c r="H3" t="str">
+      <c r="I3" t="str">
         <v>/login</v>
       </c>
     </row>
@@ -508,12 +518,15 @@
         <v/>
       </c>
       <c r="F4" t="str">
+        <v>INFO</v>
+      </c>
+      <c r="G4" t="str">
         <v>돌아가기</v>
       </c>
-      <c r="G4" t="str">
+      <c r="H4" t="str">
         <v>BACK</v>
       </c>
-      <c r="H4" t="str">
+      <c r="I4" t="str">
         <v/>
       </c>
     </row>
@@ -534,12 +547,15 @@
         <v/>
       </c>
       <c r="F5" t="str">
+        <v>ERROR</v>
+      </c>
+      <c r="G5" t="str">
         <v>다시 시도</v>
       </c>
-      <c r="G5" t="str">
+      <c r="H5" t="str">
         <v>RETRY</v>
       </c>
-      <c r="H5" t="str">
+      <c r="I5" t="str">
         <v/>
       </c>
     </row>
@@ -560,25 +576,28 @@
         <v/>
       </c>
       <c r="F6" t="str">
+        <v>CRITICAL</v>
+      </c>
+      <c r="G6" t="str">
         <v>돌아가기</v>
       </c>
-      <c r="G6" t="str">
+      <c r="H6" t="str">
         <v>BACK</v>
       </c>
-      <c r="H6" t="str">
+      <c r="I6" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I6"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -588,9 +607,10 @@
     <col min="3" max="3" width="40.83203125" customWidth="1"/>
     <col min="4" max="4" width="17.83203125" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -610,12 +630,15 @@
         <v>image</v>
       </c>
       <c r="F1" t="str">
+        <v>severity</v>
+      </c>
+      <c r="G1" t="str">
         <v>actionLabel</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>actionType</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>actionTarget</v>
       </c>
     </row>
@@ -636,12 +659,15 @@
         <v/>
       </c>
       <c r="F2" t="str">
+        <v>WARNING</v>
+      </c>
+      <c r="G2" t="str">
         <v>Retry</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" t="str">
         <v>RETRY</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
         <v/>
       </c>
     </row>
@@ -662,12 +688,15 @@
         <v/>
       </c>
       <c r="F3" t="str">
+        <v>ERROR</v>
+      </c>
+      <c r="G3" t="str">
         <v>Login</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" t="str">
         <v>REDIRECT</v>
       </c>
-      <c r="H3" t="str">
+      <c r="I3" t="str">
         <v>/login</v>
       </c>
     </row>
@@ -688,12 +717,15 @@
         <v/>
       </c>
       <c r="F4" t="str">
+        <v>INFO</v>
+      </c>
+      <c r="G4" t="str">
         <v>Go Back</v>
       </c>
-      <c r="G4" t="str">
+      <c r="H4" t="str">
         <v>BACK</v>
       </c>
-      <c r="H4" t="str">
+      <c r="I4" t="str">
         <v/>
       </c>
     </row>
@@ -714,12 +746,15 @@
         <v/>
       </c>
       <c r="F5" t="str">
+        <v>ERROR</v>
+      </c>
+      <c r="G5" t="str">
         <v>Retry</v>
       </c>
-      <c r="G5" t="str">
+      <c r="H5" t="str">
         <v>RETRY</v>
       </c>
-      <c r="H5" t="str">
+      <c r="I5" t="str">
         <v/>
       </c>
     </row>
@@ -740,18 +775,21 @@
         <v/>
       </c>
       <c r="F6" t="str">
+        <v>CRITICAL</v>
+      </c>
+      <c r="G6" t="str">
         <v>Go Back</v>
       </c>
-      <c r="G6" t="str">
+      <c r="H6" t="str">
         <v>BACK</v>
       </c>
-      <c r="H6" t="str">
+      <c r="I6" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>